<commit_message>
make gear mapping table
- made STG table (should it be CFG?)
   - maps.STG_OBS_VTR_GEARMAP
- used an excel table to manually substitute where there were missing mappings from NEGEAR to SECGEAR
- created a View for the matched OBS and CATCH data for discard: maps.CAMS_OBS_CATCH
</commit_message>
<xml_diff>
--- a/CAMS/NEGEAR_GEARCODE_MAPPING.xlsx
+++ b/CAMS/NEGEAR_GEARCODE_MAPPING.xlsx
@@ -9,11 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14250"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14250" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="readme" sheetId="5" r:id="rId1"/>
+    <sheet name="sql" sheetId="4" r:id="rId2"/>
+    <sheet name="suggestions from data request" sheetId="3" r:id="rId3"/>
+    <sheet name="mashup_table" sheetId="2" r:id="rId4"/>
+    <sheet name="upload table" sheetId="6" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">mashup_table!$A$2:$F$64</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="214">
   <si>
     <t>SECGEARFISH_2</t>
   </si>
@@ -321,13 +328,358 @@
   </si>
   <si>
     <t>SECGEAR_MAPPED</t>
+  </si>
+  <si>
+    <t>GEAR_CODE</t>
+  </si>
+  <si>
+    <t>GEAR_NAME</t>
+  </si>
+  <si>
+    <t>CLASSIFICATION_NAME</t>
+  </si>
+  <si>
+    <t>DRC</t>
+  </si>
+  <si>
+    <t>DREDGE, OCEAN QUAHOG/SURF CLAM</t>
+  </si>
+  <si>
+    <t>DREDGES</t>
+  </si>
+  <si>
+    <t>DRM</t>
+  </si>
+  <si>
+    <t>DREDGE, MUSSEL</t>
+  </si>
+  <si>
+    <t>DREDGE, OTHER</t>
+  </si>
+  <si>
+    <t>DRU</t>
+  </si>
+  <si>
+    <t>DREDGE, URCHIN</t>
+  </si>
+  <si>
+    <t>DREDGE, SCALLOP-CHAIN MAT</t>
+  </si>
+  <si>
+    <t>DREDGE,SCALLOP,CHAIN MAT,MOD</t>
+  </si>
+  <si>
+    <t>DREDGE,SCALLOP,TURTLE DEFLECT</t>
+  </si>
+  <si>
+    <t>GILL NET, DRIFT,LARGE MESH</t>
+  </si>
+  <si>
+    <t>GILLNETS</t>
+  </si>
+  <si>
+    <t>GNO</t>
+  </si>
+  <si>
+    <t>GILL NET, OTHER</t>
+  </si>
+  <si>
+    <t>GNR</t>
+  </si>
+  <si>
+    <t>GILL NET, RUNAROUND</t>
+  </si>
+  <si>
+    <t>GILL NET, SINK</t>
+  </si>
+  <si>
+    <t>GILL NET, DRIFT,SMALL MESH</t>
+  </si>
+  <si>
+    <t>OTTER TRAWL, HADDOCK SEPARATOR</t>
+  </si>
+  <si>
+    <t>TRAWL</t>
+  </si>
+  <si>
+    <t>OTTER TRAWL, BEAM</t>
+  </si>
+  <si>
+    <t>OTTER TRAWL, BOTTOM,SCALLOP</t>
+  </si>
+  <si>
+    <t>OTTER TRAWL, BOTTOM,FISH</t>
+  </si>
+  <si>
+    <t>OTTER TRAWL, MIDWATER</t>
+  </si>
+  <si>
+    <t>OTTER TRAWL, BOTTOM,OTHER</t>
+  </si>
+  <si>
+    <t>OTTER TRAWL, RUHLE</t>
+  </si>
+  <si>
+    <t>OTTER TRAWL, BOTTOM,SHRIMP</t>
+  </si>
+  <si>
+    <t>OTTER TRAWL,BOTTOM,TWIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OBP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">OTTER TRAWL, LARGE MESH BELLY PANEL </t>
+  </si>
+  <si>
+    <t>PAIR TRAWL, MIDWATER</t>
+  </si>
+  <si>
+    <t>PAIR TRAWL, BOTTOM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTS </t>
+  </si>
+  <si>
+    <t>OTTER TRAWL, BOTTOM,  SHRIMP, JOINED (TWIN TRAWL)</t>
+  </si>
+  <si>
+    <t>WEI</t>
+  </si>
+  <si>
+    <t>WEIR</t>
+  </si>
+  <si>
+    <t>TRAPS</t>
+  </si>
+  <si>
+    <t>TRP</t>
+  </si>
+  <si>
+    <t>TRAP</t>
+  </si>
+  <si>
+    <t>LONGLINE</t>
+  </si>
+  <si>
+    <t>SEINE, PURSE</t>
+  </si>
+  <si>
+    <t>SEINES</t>
+  </si>
+  <si>
+    <t>SED</t>
+  </si>
+  <si>
+    <t>SEINE, DANISH</t>
+  </si>
+  <si>
+    <t>SEINE, HAUL</t>
+  </si>
+  <si>
+    <t>SEINE, SCOTTISH</t>
+  </si>
+  <si>
+    <t>STS</t>
+  </si>
+  <si>
+    <t>SEINE, STOP</t>
+  </si>
+  <si>
+    <t>POT, CRAB</t>
+  </si>
+  <si>
+    <t>POTS</t>
+  </si>
+  <si>
+    <t>PTE</t>
+  </si>
+  <si>
+    <t>POT, EEL</t>
+  </si>
+  <si>
+    <t>POT, FISH</t>
+  </si>
+  <si>
+    <t>POT, HAG</t>
+  </si>
+  <si>
+    <t>POT, LOBSTER</t>
+  </si>
+  <si>
+    <t>POT, OTHER</t>
+  </si>
+  <si>
+    <t>POT, SHRIMP</t>
+  </si>
+  <si>
+    <t>POT, CONCH/WHELK</t>
+  </si>
+  <si>
+    <t>POTS, MIXED</t>
+  </si>
+  <si>
+    <t>DIV</t>
+  </si>
+  <si>
+    <t>DIVING GEAR</t>
+  </si>
+  <si>
+    <t>DIVING GEAR </t>
+  </si>
+  <si>
+    <t>HAND LINE/ROD &amp; REEL</t>
+  </si>
+  <si>
+    <t>HANDLINE / ROD AND REEL</t>
+  </si>
+  <si>
+    <t>TGS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TROLL LINE, GREEN STICK </t>
+  </si>
+  <si>
+    <t>CST</t>
+  </si>
+  <si>
+    <t>CASTNET</t>
+  </si>
+  <si>
+    <t>OTHER</t>
+  </si>
+  <si>
+    <t>DIP</t>
+  </si>
+  <si>
+    <t>DIP NETS</t>
+  </si>
+  <si>
+    <t>FYKE NET</t>
+  </si>
+  <si>
+    <t>HARPOON</t>
+  </si>
+  <si>
+    <t>MIXED GEAR</t>
+  </si>
+  <si>
+    <t>OTHER GEAR</t>
+  </si>
+  <si>
+    <t>RAK</t>
+  </si>
+  <si>
+    <t>HAND RAKE</t>
+  </si>
+  <si>
+    <t>HAND</t>
+  </si>
+  <si>
+    <t>got a random data request which inspired this list</t>
+  </si>
+  <si>
+    <t>OBDBS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VTR  </t>
+  </si>
+  <si>
+    <t>VTR</t>
+  </si>
+  <si>
+    <t>select distinct(secgearfish_2)</t>
+  </si>
+  <si>
+    <t>, obs_negear</t>
+  </si>
+  <si>
+    <t>, gearnm</t>
+  </si>
+  <si>
+    <t>, vtr_negear</t>
+  </si>
+  <si>
+    <t>--, vtr_gear_code</t>
+  </si>
+  <si>
+    <t>--, secgearfish</t>
+  </si>
+  <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>(</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    select o.negear as obs_negear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    , o.gearnm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    , v.negear as vtr_negear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    , v.vtr_gear_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    , o.secgearfish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    , coalesce(o.secgearfish, v.vtr_gear_code) as secgearfish_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    from obdbs.obgear@NOVA o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        left join(</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            select * from maps.cfg_fvtr_gear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        ) v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        on o.negear = v.negear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">            select * from maps.cfg_vlgear </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        ) vl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        on o.negear = vl.negear</t>
+  </si>
+  <si>
+    <t>)</t>
+  </si>
+  <si>
+    <t>order by obs_negear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There exist two mapping tables for VTR, one from the NEFSC (FVTR_GEAR)  and one from GARFO (VLGEAR). </t>
+  </si>
+  <si>
+    <t>There is also a list of gears that OBS uses (OBDBS_OBGEAR) which has different options.</t>
+  </si>
+  <si>
+    <t>MASTER_GEAR was created for CAMS discard for the final gear groupings used in statification</t>
+  </si>
+  <si>
+    <t>mismatches between OBDBS and VTR choices in gear type neccesitate a remappign to match OBS hauls with VTR subtrips. This table is for this purpose.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -335,8 +687,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="64"/>
+      <name val="Microsoft Sans Serif"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="64"/>
+      <name val="Microsoft Sans Serif"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -346,6 +726,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -362,9 +760,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -645,10 +1049,2267 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>213</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G55"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F64"/>
+  <sheetViews>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E64"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="51.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="6" max="6" width="24" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="46" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3" t="str">
+        <f>A3</f>
+        <v>LLB</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
+      <c r="E4" t="str">
+        <f>A4</f>
+        <v>HND</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>21</v>
+      </c>
+      <c r="E5" t="str">
+        <f>A5</f>
+        <v>HND</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>30</v>
+      </c>
+      <c r="E6" t="str">
+        <f>A6</f>
+        <v>HRP</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8">
+        <v>40</v>
+      </c>
+      <c r="E8" t="str">
+        <f>A8</f>
+        <v>LLP</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>50</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>50</v>
+      </c>
+      <c r="E9" t="str">
+        <f>A9</f>
+        <v>OTF</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>51</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10">
+        <v>51</v>
+      </c>
+      <c r="E10" t="str">
+        <f>A10</f>
+        <v>OTO</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>52</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11">
+        <v>52</v>
+      </c>
+      <c r="E11" t="str">
+        <f>A11</f>
+        <v>OTC</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>53</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12">
+        <v>53</v>
+      </c>
+      <c r="E12" t="str">
+        <f>A12</f>
+        <v>OTT</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13">
+        <v>54</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13">
+        <v>54</v>
+      </c>
+      <c r="E13" t="str">
+        <f>A13</f>
+        <v>OTR</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14">
+        <v>56</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14">
+        <v>56</v>
+      </c>
+      <c r="E14" t="str">
+        <f>A14</f>
+        <v>PTB</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15">
+        <v>57</v>
+      </c>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15">
+        <v>57</v>
+      </c>
+      <c r="E15" t="str">
+        <f>A15</f>
+        <v>OHS</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16">
+        <v>58</v>
+      </c>
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16">
+        <v>58</v>
+      </c>
+      <c r="E16" t="str">
+        <f>A16</f>
+        <v>OTS</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17">
+        <v>60</v>
+      </c>
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17">
+        <v>60</v>
+      </c>
+      <c r="E17" t="str">
+        <f>A17</f>
+        <v>OTH</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18">
+        <v>70</v>
+      </c>
+      <c r="C18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18">
+        <v>70</v>
+      </c>
+      <c r="E18" t="str">
+        <f>A18</f>
+        <v>SEH</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19">
+        <v>71</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19">
+        <v>71</v>
+      </c>
+      <c r="E19" t="str">
+        <f>A19</f>
+        <v>SEH</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20">
+        <v>100</v>
+      </c>
+      <c r="C20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20">
+        <v>100</v>
+      </c>
+      <c r="E20" t="str">
+        <f>A20</f>
+        <v>GNS</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>102</v>
+      </c>
+      <c r="C21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" t="s">
+        <v>35</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22">
+        <v>105</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22">
+        <v>105</v>
+      </c>
+      <c r="E22" t="str">
+        <f>A22</f>
+        <v>GNS</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23">
+        <v>110</v>
+      </c>
+      <c r="C23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23">
+        <v>110</v>
+      </c>
+      <c r="E23" t="str">
+        <f>A23</f>
+        <v>GNT</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24">
+        <v>115</v>
+      </c>
+      <c r="C24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24">
+        <v>115</v>
+      </c>
+      <c r="E24" t="str">
+        <f>A24</f>
+        <v>GND</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>116</v>
+      </c>
+      <c r="C25" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" t="s">
+        <v>41</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26">
+        <v>117</v>
+      </c>
+      <c r="C26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26">
+        <v>117</v>
+      </c>
+      <c r="E26" t="str">
+        <f>A26</f>
+        <v>GNS</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27">
+        <v>120</v>
+      </c>
+      <c r="C27" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27">
+        <v>120</v>
+      </c>
+      <c r="E27" t="str">
+        <f>A27</f>
+        <v>PUR</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>121</v>
+      </c>
+      <c r="C28" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>122</v>
+      </c>
+      <c r="C29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" t="s">
+        <v>45</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>123</v>
+      </c>
+      <c r="C30" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="1"/>
+      <c r="E30" t="s">
+        <v>45</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>124</v>
+      </c>
+      <c r="C31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" t="s">
+        <v>45</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32">
+        <v>132</v>
+      </c>
+      <c r="C32" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32">
+        <v>132</v>
+      </c>
+      <c r="E32" t="str">
+        <f>A32</f>
+        <v>DRS</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33">
+        <v>132</v>
+      </c>
+      <c r="C33" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33">
+        <v>132</v>
+      </c>
+      <c r="E33" t="s">
+        <v>51</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34">
+        <v>132</v>
+      </c>
+      <c r="C34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D34">
+        <v>132</v>
+      </c>
+      <c r="E34" t="s">
+        <v>51</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35">
+        <v>132</v>
+      </c>
+      <c r="C35" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35">
+        <v>132</v>
+      </c>
+      <c r="E35" t="s">
+        <v>51</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>142</v>
+      </c>
+      <c r="C36" t="s">
+        <v>56</v>
+      </c>
+      <c r="D36" s="1"/>
+      <c r="E36" t="s">
+        <v>30</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>57</v>
+      </c>
+      <c r="B37">
+        <v>150</v>
+      </c>
+      <c r="C37" t="s">
+        <v>58</v>
+      </c>
+      <c r="D37">
+        <v>150</v>
+      </c>
+      <c r="E37" t="str">
+        <f>A37</f>
+        <v>OBP</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38">
+        <v>170</v>
+      </c>
+      <c r="C38" t="s">
+        <v>60</v>
+      </c>
+      <c r="D38">
+        <v>170</v>
+      </c>
+      <c r="E38" t="str">
+        <f>A38</f>
+        <v>PTM</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39">
+        <v>180</v>
+      </c>
+      <c r="C39" t="s">
+        <v>62</v>
+      </c>
+      <c r="D39">
+        <v>180</v>
+      </c>
+      <c r="E39" t="s">
+        <v>63</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40">
+        <v>180</v>
+      </c>
+      <c r="C40" t="s">
+        <v>62</v>
+      </c>
+      <c r="D40">
+        <v>180</v>
+      </c>
+      <c r="E40" s="1" t="str">
+        <f>A40</f>
+        <v>PTO</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>64</v>
+      </c>
+      <c r="B41">
+        <v>180</v>
+      </c>
+      <c r="C41" t="s">
+        <v>62</v>
+      </c>
+      <c r="D41">
+        <v>180</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>61</v>
+      </c>
+      <c r="B42">
+        <v>181</v>
+      </c>
+      <c r="C42" t="s">
+        <v>65</v>
+      </c>
+      <c r="D42">
+        <v>181</v>
+      </c>
+      <c r="E42" t="str">
+        <f>A42</f>
+        <v>PTF</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>66</v>
+      </c>
+      <c r="B43">
+        <v>183</v>
+      </c>
+      <c r="C43" t="s">
+        <v>67</v>
+      </c>
+      <c r="D43">
+        <v>183</v>
+      </c>
+      <c r="E43" t="str">
+        <f>A43</f>
+        <v>PTW</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>68</v>
+      </c>
+      <c r="B44">
+        <v>186</v>
+      </c>
+      <c r="C44" t="s">
+        <v>69</v>
+      </c>
+      <c r="D44">
+        <v>186</v>
+      </c>
+      <c r="E44" t="str">
+        <f>A44</f>
+        <v>PTH</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>70</v>
+      </c>
+      <c r="B45">
+        <v>190</v>
+      </c>
+      <c r="C45" t="s">
+        <v>71</v>
+      </c>
+      <c r="D45">
+        <v>190</v>
+      </c>
+      <c r="E45" t="str">
+        <f>A45</f>
+        <v>PTS</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>72</v>
+      </c>
+      <c r="B46">
+        <v>200</v>
+      </c>
+      <c r="C46" t="s">
+        <v>73</v>
+      </c>
+      <c r="D46">
+        <v>200</v>
+      </c>
+      <c r="E46" t="str">
+        <f>A46</f>
+        <v>PTL</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>203</v>
+      </c>
+      <c r="C47" t="s">
+        <v>74</v>
+      </c>
+      <c r="D47" s="1"/>
+      <c r="E47" t="s">
+        <v>63</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>206</v>
+      </c>
+      <c r="C48" t="s">
+        <v>75</v>
+      </c>
+      <c r="D48" s="1"/>
+      <c r="E48" t="s">
+        <v>63</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>72</v>
+      </c>
+      <c r="B49">
+        <v>210</v>
+      </c>
+      <c r="C49" t="s">
+        <v>76</v>
+      </c>
+      <c r="D49">
+        <v>210</v>
+      </c>
+      <c r="E49" t="str">
+        <f>A49</f>
+        <v>PTL</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>63</v>
+      </c>
+      <c r="B50">
+        <v>210</v>
+      </c>
+      <c r="C50" t="s">
+        <v>76</v>
+      </c>
+      <c r="D50">
+        <v>210</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>77</v>
+      </c>
+      <c r="B51">
+        <v>300</v>
+      </c>
+      <c r="C51" t="s">
+        <v>78</v>
+      </c>
+      <c r="D51">
+        <v>300</v>
+      </c>
+      <c r="E51" t="str">
+        <f>A51</f>
+        <v>PTC</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>77</v>
+      </c>
+      <c r="B52">
+        <v>301</v>
+      </c>
+      <c r="C52" t="s">
+        <v>79</v>
+      </c>
+      <c r="D52">
+        <v>301</v>
+      </c>
+      <c r="E52" t="str">
+        <f>A52</f>
+        <v>PTC</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>80</v>
+      </c>
+      <c r="B53">
+        <v>320</v>
+      </c>
+      <c r="C53" t="s">
+        <v>81</v>
+      </c>
+      <c r="D53">
+        <v>320</v>
+      </c>
+      <c r="E53" t="str">
+        <f>A53</f>
+        <v>FYK</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>82</v>
+      </c>
+      <c r="B54">
+        <v>350</v>
+      </c>
+      <c r="C54" t="s">
+        <v>83</v>
+      </c>
+      <c r="D54">
+        <v>350</v>
+      </c>
+      <c r="E54" t="str">
+        <f>A54</f>
+        <v>OTB</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>352</v>
+      </c>
+      <c r="C55" t="s">
+        <v>84</v>
+      </c>
+      <c r="D55" s="1"/>
+      <c r="E55" t="s">
+        <v>82</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <v>353</v>
+      </c>
+      <c r="C56" t="s">
+        <v>85</v>
+      </c>
+      <c r="D56" s="1"/>
+      <c r="E56" t="s">
+        <v>82</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>86</v>
+      </c>
+      <c r="B57">
+        <v>360</v>
+      </c>
+      <c r="C57" t="s">
+        <v>87</v>
+      </c>
+      <c r="D57">
+        <v>360</v>
+      </c>
+      <c r="E57" t="str">
+        <f>A57</f>
+        <v>SES</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>88</v>
+      </c>
+      <c r="B58">
+        <v>370</v>
+      </c>
+      <c r="C58" t="s">
+        <v>89</v>
+      </c>
+      <c r="D58">
+        <v>370</v>
+      </c>
+      <c r="E58" t="str">
+        <f>A58</f>
+        <v>OTM</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>90</v>
+      </c>
+      <c r="B59">
+        <v>381</v>
+      </c>
+      <c r="C59" t="s">
+        <v>91</v>
+      </c>
+      <c r="D59">
+        <v>381</v>
+      </c>
+      <c r="E59" t="str">
+        <f>A59</f>
+        <v>DRO</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B60">
+        <v>383</v>
+      </c>
+      <c r="C60" t="s">
+        <v>92</v>
+      </c>
+      <c r="D60" s="1"/>
+      <c r="E60" t="s">
+        <v>90</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>90</v>
+      </c>
+      <c r="B61">
+        <v>386</v>
+      </c>
+      <c r="C61" t="s">
+        <v>93</v>
+      </c>
+      <c r="D61">
+        <v>386</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>94</v>
+      </c>
+      <c r="B62">
+        <v>450</v>
+      </c>
+      <c r="C62" t="s">
+        <v>95</v>
+      </c>
+      <c r="D62">
+        <v>450</v>
+      </c>
+      <c r="E62" t="str">
+        <f>A62</f>
+        <v>TTS</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>96</v>
+      </c>
+      <c r="B63">
+        <v>999</v>
+      </c>
+      <c r="C63" t="s">
+        <v>97</v>
+      </c>
+      <c r="D63" s="1">
+        <v>999</v>
+      </c>
+      <c r="E63" t="s">
+        <v>30</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>30</v>
+      </c>
+      <c r="B64">
+        <v>999</v>
+      </c>
+      <c r="C64" t="s">
+        <v>97</v>
+      </c>
+      <c r="D64">
+        <v>999</v>
+      </c>
+      <c r="E64" t="str">
+        <f>A64</f>
+        <v>OTH</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A2:F64">
+    <sortState ref="A3:F64">
+      <sortCondition ref="B2:B64"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46:E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,7 +3318,7 @@
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="51.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -673,7 +3334,7 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="5" t="s">
         <v>98</v>
       </c>
     </row>
@@ -709,7 +3370,7 @@
         <v>20</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E63" si="0">A3</f>
+        <f>A3</f>
         <v>HND</v>
       </c>
     </row>
@@ -727,7 +3388,7 @@
         <v>21</v>
       </c>
       <c r="E4" t="str">
-        <f t="shared" si="0"/>
+        <f>A4</f>
         <v>HND</v>
       </c>
     </row>
@@ -745,7 +3406,7 @@
         <v>30</v>
       </c>
       <c r="E5" t="str">
-        <f t="shared" si="0"/>
+        <f>A5</f>
         <v>HRP</v>
       </c>
     </row>
@@ -775,7 +3436,7 @@
         <v>40</v>
       </c>
       <c r="E7" t="str">
-        <f t="shared" si="0"/>
+        <f>A7</f>
         <v>LLP</v>
       </c>
     </row>
@@ -793,7 +3454,7 @@
         <v>50</v>
       </c>
       <c r="E8" t="str">
-        <f t="shared" si="0"/>
+        <f>A8</f>
         <v>OTF</v>
       </c>
     </row>
@@ -811,7 +3472,7 @@
         <v>51</v>
       </c>
       <c r="E9" t="str">
-        <f t="shared" si="0"/>
+        <f>A9</f>
         <v>OTO</v>
       </c>
     </row>
@@ -829,7 +3490,7 @@
         <v>52</v>
       </c>
       <c r="E10" t="str">
-        <f t="shared" si="0"/>
+        <f>A10</f>
         <v>OTC</v>
       </c>
     </row>
@@ -847,7 +3508,7 @@
         <v>53</v>
       </c>
       <c r="E11" t="str">
-        <f t="shared" si="0"/>
+        <f>A11</f>
         <v>OTT</v>
       </c>
     </row>
@@ -865,7 +3526,7 @@
         <v>54</v>
       </c>
       <c r="E12" t="str">
-        <f t="shared" si="0"/>
+        <f>A12</f>
         <v>OTR</v>
       </c>
     </row>
@@ -883,7 +3544,7 @@
         <v>56</v>
       </c>
       <c r="E13" t="str">
-        <f t="shared" si="0"/>
+        <f>A13</f>
         <v>PTB</v>
       </c>
     </row>
@@ -901,7 +3562,7 @@
         <v>57</v>
       </c>
       <c r="E14" t="str">
-        <f t="shared" si="0"/>
+        <f>A14</f>
         <v>OHS</v>
       </c>
     </row>
@@ -919,7 +3580,7 @@
         <v>58</v>
       </c>
       <c r="E15" t="str">
-        <f t="shared" si="0"/>
+        <f>A15</f>
         <v>OTS</v>
       </c>
     </row>
@@ -937,7 +3598,7 @@
         <v>60</v>
       </c>
       <c r="E16" t="str">
-        <f t="shared" si="0"/>
+        <f>A16</f>
         <v>OTH</v>
       </c>
     </row>
@@ -955,7 +3616,7 @@
         <v>70</v>
       </c>
       <c r="E17" t="str">
-        <f t="shared" si="0"/>
+        <f>A17</f>
         <v>SEH</v>
       </c>
     </row>
@@ -973,7 +3634,7 @@
         <v>71</v>
       </c>
       <c r="E18" t="str">
-        <f t="shared" si="0"/>
+        <f>A18</f>
         <v>SEH</v>
       </c>
     </row>
@@ -991,7 +3652,7 @@
         <v>100</v>
       </c>
       <c r="E19" t="str">
-        <f t="shared" si="0"/>
+        <f>A19</f>
         <v>GNS</v>
       </c>
     </row>
@@ -1021,7 +3682,7 @@
         <v>105</v>
       </c>
       <c r="E21" t="str">
-        <f t="shared" si="0"/>
+        <f>A21</f>
         <v>GNS</v>
       </c>
     </row>
@@ -1039,7 +3700,7 @@
         <v>110</v>
       </c>
       <c r="E22" t="str">
-        <f t="shared" si="0"/>
+        <f>A22</f>
         <v>GNT</v>
       </c>
     </row>
@@ -1057,7 +3718,7 @@
         <v>115</v>
       </c>
       <c r="E23" t="str">
-        <f t="shared" si="0"/>
+        <f>A23</f>
         <v>GND</v>
       </c>
     </row>
@@ -1087,7 +3748,7 @@
         <v>117</v>
       </c>
       <c r="E25" t="str">
-        <f t="shared" si="0"/>
+        <f>A25</f>
         <v>GNS</v>
       </c>
     </row>
@@ -1105,7 +3766,7 @@
         <v>120</v>
       </c>
       <c r="E26" t="str">
-        <f t="shared" si="0"/>
+        <f>A26</f>
         <v>PUR</v>
       </c>
     </row>
@@ -1171,7 +3832,7 @@
         <v>132</v>
       </c>
       <c r="E31" t="str">
-        <f t="shared" si="0"/>
+        <f>A31</f>
         <v>DRS</v>
       </c>
     </row>
@@ -1252,7 +3913,7 @@
         <v>150</v>
       </c>
       <c r="E36" t="str">
-        <f t="shared" si="0"/>
+        <f>A36</f>
         <v>OBP</v>
       </c>
     </row>
@@ -1270,7 +3931,7 @@
         <v>170</v>
       </c>
       <c r="E37" t="str">
-        <f t="shared" si="0"/>
+        <f>A37</f>
         <v>PTM</v>
       </c>
     </row>
@@ -1287,9 +3948,8 @@
       <c r="D38">
         <v>180</v>
       </c>
-      <c r="E38" t="str">
-        <f t="shared" si="0"/>
-        <v>PTF</v>
+      <c r="E38" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1305,8 +3965,8 @@
       <c r="D39">
         <v>180</v>
       </c>
-      <c r="E39" t="str">
-        <f t="shared" si="0"/>
+      <c r="E39" s="1" t="str">
+        <f>A39</f>
         <v>PTO</v>
       </c>
     </row>
@@ -1323,9 +3983,8 @@
       <c r="D40">
         <v>180</v>
       </c>
-      <c r="E40" t="str">
-        <f t="shared" si="0"/>
-        <v>PTX</v>
+      <c r="E40" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1342,7 +4001,7 @@
         <v>181</v>
       </c>
       <c r="E41" t="str">
-        <f t="shared" si="0"/>
+        <f>A41</f>
         <v>PTF</v>
       </c>
     </row>
@@ -1360,7 +4019,7 @@
         <v>183</v>
       </c>
       <c r="E42" t="str">
-        <f t="shared" si="0"/>
+        <f>A42</f>
         <v>PTW</v>
       </c>
     </row>
@@ -1378,7 +4037,7 @@
         <v>186</v>
       </c>
       <c r="E43" t="str">
-        <f t="shared" si="0"/>
+        <f>A43</f>
         <v>PTH</v>
       </c>
     </row>
@@ -1396,7 +4055,7 @@
         <v>190</v>
       </c>
       <c r="E44" t="str">
-        <f t="shared" si="0"/>
+        <f>A44</f>
         <v>PTS</v>
       </c>
     </row>
@@ -1414,7 +4073,7 @@
         <v>200</v>
       </c>
       <c r="E45" t="str">
-        <f t="shared" si="0"/>
+        <f>A45</f>
         <v>PTL</v>
       </c>
     </row>
@@ -1426,8 +4085,8 @@
         <v>74</v>
       </c>
       <c r="D46" s="1"/>
-      <c r="E46" t="s">
-        <v>63</v>
+      <c r="E46" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1438,8 +4097,8 @@
         <v>75</v>
       </c>
       <c r="D47" s="1"/>
-      <c r="E47" t="s">
-        <v>63</v>
+      <c r="E47" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1456,7 +4115,7 @@
         <v>210</v>
       </c>
       <c r="E48" t="str">
-        <f t="shared" si="0"/>
+        <f>A48</f>
         <v>PTL</v>
       </c>
     </row>
@@ -1473,9 +4132,8 @@
       <c r="D49">
         <v>210</v>
       </c>
-      <c r="E49" t="str">
-        <f t="shared" si="0"/>
-        <v>PTO</v>
+      <c r="E49" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1492,7 +4150,7 @@
         <v>300</v>
       </c>
       <c r="E50" t="str">
-        <f t="shared" si="0"/>
+        <f>A50</f>
         <v>PTC</v>
       </c>
     </row>
@@ -1510,7 +4168,7 @@
         <v>301</v>
       </c>
       <c r="E51" t="str">
-        <f t="shared" si="0"/>
+        <f>A51</f>
         <v>PTC</v>
       </c>
     </row>
@@ -1528,7 +4186,7 @@
         <v>320</v>
       </c>
       <c r="E52" t="str">
-        <f t="shared" si="0"/>
+        <f>A52</f>
         <v>FYK</v>
       </c>
     </row>
@@ -1546,7 +4204,7 @@
         <v>350</v>
       </c>
       <c r="E53" t="str">
-        <f t="shared" si="0"/>
+        <f>A53</f>
         <v>OTB</v>
       </c>
     </row>
@@ -1588,7 +4246,7 @@
         <v>360</v>
       </c>
       <c r="E56" t="str">
-        <f t="shared" si="0"/>
+        <f>A56</f>
         <v>SES</v>
       </c>
     </row>
@@ -1606,7 +4264,7 @@
         <v>370</v>
       </c>
       <c r="E57" t="str">
-        <f t="shared" si="0"/>
+        <f>A57</f>
         <v>OTM</v>
       </c>
     </row>
@@ -1624,7 +4282,7 @@
         <v>381</v>
       </c>
       <c r="E58" t="str">
-        <f t="shared" si="0"/>
+        <f>A58</f>
         <v>DRO</v>
       </c>
     </row>
@@ -1653,9 +4311,8 @@
       <c r="D60">
         <v>386</v>
       </c>
-      <c r="E60" t="str">
-        <f t="shared" si="0"/>
-        <v>DRO</v>
+      <c r="E60" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -1672,7 +4329,7 @@
         <v>450</v>
       </c>
       <c r="E61" t="str">
-        <f t="shared" si="0"/>
+        <f>A61</f>
         <v>TTS</v>
       </c>
     </row>
@@ -1707,7 +4364,7 @@
         <v>999</v>
       </c>
       <c r="E63" t="str">
-        <f t="shared" si="0"/>
+        <f>A63</f>
         <v>OTH</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated SECGEAR_MAPPED staging table
NEGEAR 400 is not in OBDBS.OBGEAR so was not included in the gear mapping. updated this manually in excel sheet
rebuilt staging table
rebuilt MAPS.CAMS_OBS_CATCH
</commit_message>
<xml_diff>
--- a/CAMS/NEGEAR_GEARCODE_MAPPING.xlsx
+++ b/CAMS/NEGEAR_GEARCODE_MAPPING.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="215">
   <si>
     <t>SECGEARFISH_2</t>
   </si>
@@ -673,6 +673,9 @@
   </si>
   <si>
     <t>mismatches between OBDBS and VTR choices in gear type neccesitate a remappign to match OBS hauls with VTR subtrips. This table is for this purpose.</t>
+  </si>
+  <si>
+    <t>DREDGE, CLAM</t>
   </si>
 </sst>
 </file>
@@ -2190,7 +2193,7 @@
         <v>40</v>
       </c>
       <c r="E8" t="str">
-        <f>A8</f>
+        <f t="shared" ref="E8:E20" si="0">A8</f>
         <v>LLP</v>
       </c>
       <c r="F8" s="3" t="s">
@@ -2211,7 +2214,7 @@
         <v>50</v>
       </c>
       <c r="E9" t="str">
-        <f>A9</f>
+        <f t="shared" si="0"/>
         <v>OTF</v>
       </c>
       <c r="F9" s="3" t="s">
@@ -2232,7 +2235,7 @@
         <v>51</v>
       </c>
       <c r="E10" t="str">
-        <f>A10</f>
+        <f t="shared" si="0"/>
         <v>OTO</v>
       </c>
       <c r="F10" s="3" t="s">
@@ -2253,7 +2256,7 @@
         <v>52</v>
       </c>
       <c r="E11" t="str">
-        <f>A11</f>
+        <f t="shared" si="0"/>
         <v>OTC</v>
       </c>
       <c r="F11" s="3" t="s">
@@ -2274,7 +2277,7 @@
         <v>53</v>
       </c>
       <c r="E12" t="str">
-        <f>A12</f>
+        <f t="shared" si="0"/>
         <v>OTT</v>
       </c>
       <c r="F12" s="3" t="s">
@@ -2295,7 +2298,7 @@
         <v>54</v>
       </c>
       <c r="E13" t="str">
-        <f>A13</f>
+        <f t="shared" si="0"/>
         <v>OTR</v>
       </c>
       <c r="F13" s="3" t="s">
@@ -2316,7 +2319,7 @@
         <v>56</v>
       </c>
       <c r="E14" t="str">
-        <f>A14</f>
+        <f t="shared" si="0"/>
         <v>PTB</v>
       </c>
       <c r="F14" s="3" t="s">
@@ -2337,7 +2340,7 @@
         <v>57</v>
       </c>
       <c r="E15" t="str">
-        <f>A15</f>
+        <f t="shared" si="0"/>
         <v>OHS</v>
       </c>
       <c r="F15" s="3" t="s">
@@ -2358,7 +2361,7 @@
         <v>58</v>
       </c>
       <c r="E16" t="str">
-        <f>A16</f>
+        <f t="shared" si="0"/>
         <v>OTS</v>
       </c>
       <c r="F16" s="3" t="s">
@@ -2379,7 +2382,7 @@
         <v>60</v>
       </c>
       <c r="E17" t="str">
-        <f>A17</f>
+        <f t="shared" si="0"/>
         <v>OTH</v>
       </c>
       <c r="F17" s="3" t="s">
@@ -2400,7 +2403,7 @@
         <v>70</v>
       </c>
       <c r="E18" t="str">
-        <f>A18</f>
+        <f t="shared" si="0"/>
         <v>SEH</v>
       </c>
       <c r="F18" s="4" t="s">
@@ -2421,7 +2424,7 @@
         <v>71</v>
       </c>
       <c r="E19" t="str">
-        <f>A19</f>
+        <f t="shared" si="0"/>
         <v>SEH</v>
       </c>
       <c r="F19" s="4" t="s">
@@ -2442,7 +2445,7 @@
         <v>100</v>
       </c>
       <c r="E20" t="str">
-        <f>A20</f>
+        <f t="shared" si="0"/>
         <v>GNS</v>
       </c>
       <c r="F20" s="4" t="s">
@@ -3306,10 +3309,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46:E47"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3436,7 +3439,7 @@
         <v>40</v>
       </c>
       <c r="E7" t="str">
-        <f>A7</f>
+        <f t="shared" ref="E7:E19" si="0">A7</f>
         <v>LLP</v>
       </c>
     </row>
@@ -3454,7 +3457,7 @@
         <v>50</v>
       </c>
       <c r="E8" t="str">
-        <f>A8</f>
+        <f t="shared" si="0"/>
         <v>OTF</v>
       </c>
     </row>
@@ -3472,7 +3475,7 @@
         <v>51</v>
       </c>
       <c r="E9" t="str">
-        <f>A9</f>
+        <f t="shared" si="0"/>
         <v>OTO</v>
       </c>
     </row>
@@ -3490,7 +3493,7 @@
         <v>52</v>
       </c>
       <c r="E10" t="str">
-        <f>A10</f>
+        <f t="shared" si="0"/>
         <v>OTC</v>
       </c>
     </row>
@@ -3508,7 +3511,7 @@
         <v>53</v>
       </c>
       <c r="E11" t="str">
-        <f>A11</f>
+        <f t="shared" si="0"/>
         <v>OTT</v>
       </c>
     </row>
@@ -3526,7 +3529,7 @@
         <v>54</v>
       </c>
       <c r="E12" t="str">
-        <f>A12</f>
+        <f t="shared" si="0"/>
         <v>OTR</v>
       </c>
     </row>
@@ -3544,7 +3547,7 @@
         <v>56</v>
       </c>
       <c r="E13" t="str">
-        <f>A13</f>
+        <f t="shared" si="0"/>
         <v>PTB</v>
       </c>
     </row>
@@ -3562,7 +3565,7 @@
         <v>57</v>
       </c>
       <c r="E14" t="str">
-        <f>A14</f>
+        <f t="shared" si="0"/>
         <v>OHS</v>
       </c>
     </row>
@@ -3580,7 +3583,7 @@
         <v>58</v>
       </c>
       <c r="E15" t="str">
-        <f>A15</f>
+        <f t="shared" si="0"/>
         <v>OTS</v>
       </c>
     </row>
@@ -3598,7 +3601,7 @@
         <v>60</v>
       </c>
       <c r="E16" t="str">
-        <f>A16</f>
+        <f t="shared" si="0"/>
         <v>OTH</v>
       </c>
     </row>
@@ -3616,7 +3619,7 @@
         <v>70</v>
       </c>
       <c r="E17" t="str">
-        <f>A17</f>
+        <f t="shared" si="0"/>
         <v>SEH</v>
       </c>
     </row>
@@ -3634,7 +3637,7 @@
         <v>71</v>
       </c>
       <c r="E18" t="str">
-        <f>A18</f>
+        <f t="shared" si="0"/>
         <v>SEH</v>
       </c>
     </row>
@@ -3652,7 +3655,7 @@
         <v>100</v>
       </c>
       <c r="E19" t="str">
-        <f>A19</f>
+        <f t="shared" si="0"/>
         <v>GNS</v>
       </c>
     </row>
@@ -4299,17 +4302,14 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>90</v>
-      </c>
       <c r="B60">
-        <v>386</v>
+        <v>400</v>
       </c>
       <c r="C60" t="s">
-        <v>93</v>
+        <v>214</v>
       </c>
       <c r="D60">
-        <v>386</v>
+        <v>400</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>102</v>
@@ -4317,42 +4317,42 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B61">
-        <v>450</v>
+        <v>386</v>
       </c>
       <c r="C61" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D61">
-        <v>450</v>
-      </c>
-      <c r="E61" t="str">
-        <f>A61</f>
-        <v>TTS</v>
+        <v>386</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B62">
-        <v>999</v>
+        <v>450</v>
       </c>
       <c r="C62" t="s">
-        <v>97</v>
-      </c>
-      <c r="D62" s="1">
-        <v>999</v>
-      </c>
-      <c r="E62" t="s">
-        <v>30</v>
+        <v>95</v>
+      </c>
+      <c r="D62">
+        <v>450</v>
+      </c>
+      <c r="E62" t="str">
+        <f>A62</f>
+        <v>TTS</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>30</v>
+        <v>96</v>
       </c>
       <c r="B63">
         <v>999</v>
@@ -4360,11 +4360,28 @@
       <c r="C63" t="s">
         <v>97</v>
       </c>
-      <c r="D63">
+      <c r="D63" s="1">
         <v>999</v>
       </c>
-      <c r="E63" t="str">
-        <f>A63</f>
+      <c r="E63" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>30</v>
+      </c>
+      <c r="B64">
+        <v>999</v>
+      </c>
+      <c r="C64" t="s">
+        <v>97</v>
+      </c>
+      <c r="D64">
+        <v>999</v>
+      </c>
+      <c r="E64" t="str">
+        <f>A64</f>
         <v>OTH</v>
       </c>
     </row>

</xml_diff>